<commit_message>
Scripts de pricing diario 2015-2024 y pricing diario histórico.
</commit_message>
<xml_diff>
--- a/Datos limpios/Pricing diario/2025/Cebada.xlsx
+++ b/Datos limpios/Pricing diario/2025/Cebada.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J213"/>
+  <dimension ref="A1:K213"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +415,11 @@
           <t>TOTAL</t>
         </is>
       </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>PRODUCTO</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2">
@@ -447,6 +452,11 @@
       <c r="J2">
         <v>775</v>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2">
@@ -479,6 +489,11 @@
       <c r="J3">
         <v>23000.05</v>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2">
@@ -511,6 +526,11 @@
       <c r="J4">
         <v>41543.73</v>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2">
@@ -543,6 +563,11 @@
       <c r="J5">
         <v>40869.25</v>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2">
@@ -575,6 +600,11 @@
       <c r="J6">
         <v>66766.60000000001</v>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2">
@@ -607,6 +637,11 @@
       <c r="J7">
         <v>32684.07</v>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2">
@@ -639,6 +674,11 @@
       <c r="J8">
         <v>36384.81</v>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2">
@@ -671,6 +711,11 @@
       <c r="J9">
         <v>32367.8</v>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2">
@@ -703,6 +748,11 @@
       <c r="J10">
         <v>10006.76</v>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2">
@@ -735,6 +785,11 @@
       <c r="J11">
         <v>73816.70999999999</v>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2">
@@ -767,6 +822,11 @@
       <c r="J12">
         <v>54022.68</v>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2">
@@ -799,6 +859,11 @@
       <c r="J13">
         <v>88700.02</v>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2">
@@ -831,6 +896,11 @@
       <c r="J14">
         <v>17604.14</v>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2">
@@ -863,6 +933,11 @@
       <c r="J15">
         <v>42702.74</v>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2">
@@ -895,6 +970,11 @@
       <c r="J16">
         <v>120097.03</v>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2">
@@ -927,6 +1007,11 @@
       <c r="J17">
         <v>41002.46</v>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2">
@@ -959,6 +1044,11 @@
       <c r="J18">
         <v>23623.45</v>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2">
@@ -991,6 +1081,11 @@
       <c r="J19">
         <v>17407</v>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2">
@@ -1023,6 +1118,11 @@
       <c r="J20">
         <v>19872.26</v>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2">
@@ -1055,6 +1155,11 @@
       <c r="J21">
         <v>27814.2</v>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2">
@@ -1087,6 +1192,11 @@
       <c r="J22">
         <v>28746.97</v>
       </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2">
@@ -1119,6 +1229,11 @@
       <c r="J23">
         <v>17883.21</v>
       </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2">
@@ -1151,6 +1266,11 @@
       <c r="J24">
         <v>22586.57</v>
       </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2">
@@ -1183,6 +1303,11 @@
       <c r="J25">
         <v>20</v>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2">
@@ -1215,6 +1340,11 @@
       <c r="J26">
         <v>48319.03</v>
       </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2">
@@ -1247,6 +1377,11 @@
       <c r="J27">
         <v>29393.16</v>
       </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2">
@@ -1279,6 +1414,11 @@
       <c r="J28">
         <v>24253.72</v>
       </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2">
@@ -1311,6 +1451,11 @@
       <c r="J29">
         <v>21949.63</v>
       </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2">
@@ -1343,6 +1488,11 @@
       <c r="J30">
         <v>21760.38</v>
       </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2">
@@ -1375,6 +1525,11 @@
       <c r="J31">
         <v>22548.78</v>
       </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2">
@@ -1407,6 +1562,11 @@
       <c r="J32">
         <v>48621.53</v>
       </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2">
@@ -1439,6 +1599,11 @@
       <c r="J33">
         <v>36095.82</v>
       </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2">
@@ -1471,6 +1636,11 @@
       <c r="J34">
         <v>35637.35000000001</v>
       </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2">
@@ -1503,6 +1673,11 @@
       <c r="J35">
         <v>11026.2</v>
       </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2">
@@ -1535,6 +1710,11 @@
       <c r="J36">
         <v>500</v>
       </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="2">
@@ -1567,6 +1747,11 @@
       <c r="J37">
         <v>55</v>
       </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="2">
@@ -1599,6 +1784,11 @@
       <c r="J38">
         <v>64138.32</v>
       </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="2">
@@ -1631,6 +1821,11 @@
       <c r="J39">
         <v>20304.39</v>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2">
@@ -1663,6 +1858,11 @@
       <c r="J40">
         <v>18271.01</v>
       </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="2">
@@ -1695,6 +1895,11 @@
       <c r="J41">
         <v>24166.79</v>
       </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2">
@@ -1727,6 +1932,11 @@
       <c r="J42">
         <v>24307.4</v>
       </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2">
@@ -1759,6 +1969,11 @@
       <c r="J43">
         <v>17265.76</v>
       </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="2">
@@ -1791,6 +2006,11 @@
       <c r="J44">
         <v>16495.73</v>
       </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="2">
@@ -1823,6 +2043,11 @@
       <c r="J45">
         <v>33978.04</v>
       </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="2">
@@ -1855,6 +2080,11 @@
       <c r="J46">
         <v>19667.55</v>
       </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="2">
@@ -1887,6 +2117,11 @@
       <c r="J47">
         <v>14794.09</v>
       </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="2">
@@ -1919,6 +2154,11 @@
       <c r="J48">
         <v>14504.46</v>
       </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="2">
@@ -1951,6 +2191,11 @@
       <c r="J49">
         <v>18643.84</v>
       </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="2">
@@ -1983,6 +2228,11 @@
       <c r="J50">
         <v>15958.56</v>
       </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="2">
@@ -2015,6 +2265,11 @@
       <c r="J51">
         <v>19406.97</v>
       </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="2">
@@ -2047,6 +2302,11 @@
       <c r="J52">
         <v>21535.71</v>
       </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="2">
@@ -2079,6 +2339,11 @@
       <c r="J53">
         <v>6847.98</v>
       </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="2">
@@ -2111,6 +2376,11 @@
       <c r="J54">
         <v>8585.98</v>
       </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="2">
@@ -2143,6 +2413,11 @@
       <c r="J55">
         <v>12512.77</v>
       </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="2">
@@ -2175,6 +2450,11 @@
       <c r="J56">
         <v>11171.74</v>
       </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="2">
@@ -2207,6 +2487,11 @@
       <c r="J57">
         <v>8235.49</v>
       </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="2">
@@ -2239,6 +2524,11 @@
       <c r="J58">
         <v>7010.8</v>
       </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="2">
@@ -2271,6 +2561,11 @@
       <c r="J59">
         <v>12184.26</v>
       </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="2">
@@ -2303,6 +2598,11 @@
       <c r="J60">
         <v>11763.3</v>
       </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="2">
@@ -2335,6 +2635,11 @@
       <c r="J61">
         <v>2500</v>
       </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="2">
@@ -2367,6 +2672,11 @@
       <c r="J62">
         <v>15291.04</v>
       </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" s="2">
@@ -2399,6 +2709,11 @@
       <c r="J63">
         <v>10267.56</v>
       </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" s="2">
@@ -2431,6 +2746,11 @@
       <c r="J64">
         <v>7725</v>
       </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" s="2">
@@ -2463,6 +2783,11 @@
       <c r="J65">
         <v>13170.5</v>
       </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" s="2">
@@ -2495,6 +2820,11 @@
       <c r="J66">
         <v>1590</v>
       </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" s="2">
@@ -2527,6 +2857,11 @@
       <c r="J67">
         <v>-420</v>
       </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" s="2">
@@ -2559,6 +2894,11 @@
       <c r="J68">
         <v>12030.61</v>
       </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" s="2">
@@ -2591,6 +2931,11 @@
       <c r="J69">
         <v>10428.7</v>
       </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" s="2">
@@ -2623,6 +2968,11 @@
       <c r="J70">
         <v>8964.110000000001</v>
       </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" s="2">
@@ -2655,6 +3005,11 @@
       <c r="J71">
         <v>18115.09</v>
       </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" s="2">
@@ -2687,6 +3042,11 @@
       <c r="J72">
         <v>429.39</v>
       </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" s="2">
@@ -2719,6 +3079,11 @@
       <c r="J73">
         <v>8651.940000000001</v>
       </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" s="2">
@@ -2751,6 +3116,11 @@
       <c r="J74">
         <v>7749.4</v>
       </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" s="2">
@@ -2783,6 +3153,11 @@
       <c r="J75">
         <v>9115.620000000001</v>
       </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" s="2">
@@ -2815,6 +3190,11 @@
       <c r="J76">
         <v>11436.57</v>
       </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" s="2">
@@ -2847,6 +3227,11 @@
       <c r="J77">
         <v>7112.48</v>
       </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" s="2">
@@ -2879,6 +3264,11 @@
       <c r="J78">
         <v>810</v>
       </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" s="2">
@@ -2911,6 +3301,11 @@
       <c r="J79">
         <v>2283.46</v>
       </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" s="2">
@@ -2943,6 +3338,11 @@
       <c r="J80">
         <v>20940.02</v>
       </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" s="2">
@@ -2975,6 +3375,11 @@
       <c r="J81">
         <v>13791.54</v>
       </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" s="2">
@@ -3007,6 +3412,11 @@
       <c r="J82">
         <v>30</v>
       </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" s="2">
@@ -3039,6 +3449,11 @@
       <c r="J83">
         <v>9683.42</v>
       </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" s="2">
@@ -3071,6 +3486,11 @@
       <c r="J84">
         <v>8366.24</v>
       </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" s="2">
@@ -3103,6 +3523,11 @@
       <c r="J85">
         <v>15603.81</v>
       </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" s="2">
@@ -3135,6 +3560,11 @@
       <c r="J86">
         <v>13071.04</v>
       </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" s="2">
@@ -3167,6 +3597,11 @@
       <c r="J87">
         <v>11660.24</v>
       </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" s="2">
@@ -3199,6 +3634,11 @@
       <c r="J88">
         <v>28905.1</v>
       </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" s="2">
@@ -3231,6 +3671,11 @@
       <c r="J89">
         <v>51314.09</v>
       </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" s="2">
@@ -3263,6 +3708,11 @@
       <c r="J90">
         <v>9045.68</v>
       </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" s="2">
@@ -3295,6 +3745,11 @@
       <c r="J91">
         <v>60</v>
       </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" s="2">
@@ -3327,6 +3782,11 @@
       <c r="J92">
         <v>3254.61</v>
       </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" s="2">
@@ -3359,6 +3819,11 @@
       <c r="J93">
         <v>30516.32</v>
       </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" s="2">
@@ -3391,6 +3856,11 @@
       <c r="J94">
         <v>7944.94</v>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" s="2">
@@ -3423,6 +3893,11 @@
       <c r="J95">
         <v>9128.33</v>
       </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" s="2">
@@ -3455,6 +3930,11 @@
       <c r="J96">
         <v>2453.809999999999</v>
       </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" s="2">
@@ -3487,6 +3967,11 @@
       <c r="J97">
         <v>4946</v>
       </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" s="2">
@@ -3519,6 +4004,11 @@
       <c r="J98">
         <v>10341.21</v>
       </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" s="2">
@@ -3551,6 +4041,11 @@
       <c r="J99">
         <v>6660</v>
       </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" s="2">
@@ -3583,6 +4078,11 @@
       <c r="J100">
         <v>18565.4</v>
       </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" s="2">
@@ -3615,6 +4115,11 @@
       <c r="J101">
         <v>5028.32</v>
       </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" s="2">
@@ -3647,6 +4152,11 @@
       <c r="J102">
         <v>5557.3</v>
       </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" s="2">
@@ -3679,6 +4189,11 @@
       <c r="J103">
         <v>6560.46</v>
       </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" s="2">
@@ -3711,6 +4226,11 @@
       <c r="J104">
         <v>5996.54</v>
       </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" s="2">
@@ -3743,6 +4263,11 @@
       <c r="J105">
         <v>8259.34</v>
       </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" s="2">
@@ -3775,6 +4300,11 @@
       <c r="J106">
         <v>5148.25</v>
       </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" s="2">
@@ -3807,6 +4337,11 @@
       <c r="J107">
         <v>14943.86</v>
       </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" s="2">
@@ -3839,6 +4374,11 @@
       <c r="J108">
         <v>9653.73</v>
       </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" s="2">
@@ -3871,6 +4411,11 @@
       <c r="J109">
         <v>2834.86</v>
       </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" s="2">
@@ -3903,6 +4448,11 @@
       <c r="J110">
         <v>12632.13</v>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" s="2">
@@ -3935,6 +4485,11 @@
       <c r="J111">
         <v>14811.91</v>
       </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" s="2">
@@ -3967,6 +4522,11 @@
       <c r="J112">
         <v>10762.4</v>
       </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" s="2">
@@ -3999,6 +4559,11 @@
       <c r="J113">
         <v>5994.52</v>
       </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" s="2">
@@ -4031,6 +4596,11 @@
       <c r="J114">
         <v>1921.4</v>
       </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" s="2">
@@ -4063,6 +4633,11 @@
       <c r="J115">
         <v>32491.14</v>
       </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" s="2">
@@ -4095,6 +4670,11 @@
       <c r="J116">
         <v>2251.4</v>
       </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" s="2">
@@ -4127,6 +4707,11 @@
       <c r="J117">
         <v>4038.67</v>
       </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" s="2">
@@ -4159,6 +4744,11 @@
       <c r="J118">
         <v>500</v>
       </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" s="2">
@@ -4191,6 +4781,11 @@
       <c r="J119">
         <v>23442.17</v>
       </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" s="2">
@@ -4223,6 +4818,11 @@
       <c r="J120">
         <v>13976.64</v>
       </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" s="2">
@@ -4255,6 +4855,11 @@
       <c r="J121">
         <v>8848.84</v>
       </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" s="2">
@@ -4287,6 +4892,11 @@
       <c r="J122">
         <v>8870.549999999999</v>
       </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" s="2">
@@ -4319,6 +4929,11 @@
       <c r="J123">
         <v>9697.620000000001</v>
       </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" s="2">
@@ -4351,6 +4966,11 @@
       <c r="J124">
         <v>90</v>
       </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" s="2">
@@ -4383,6 +5003,11 @@
       <c r="J125">
         <v>3170</v>
       </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" s="2">
@@ -4415,6 +5040,11 @@
       <c r="J126">
         <v>3584.7</v>
       </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" s="2">
@@ -4447,6 +5077,11 @@
       <c r="J127">
         <v>2876.62</v>
       </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" s="2">
@@ -4479,6 +5114,11 @@
       <c r="J128">
         <v>15056.77</v>
       </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" s="2">
@@ -4511,6 +5151,11 @@
       <c r="J129">
         <v>8822.279999999999</v>
       </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" s="2">
@@ -4543,6 +5188,11 @@
       <c r="J130">
         <v>4150.12</v>
       </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" s="2">
@@ -4575,6 +5225,11 @@
       <c r="J131">
         <v>3296.57</v>
       </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" s="2">
@@ -4607,6 +5262,11 @@
       <c r="J132">
         <v>6355.16</v>
       </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" s="2">
@@ -4639,6 +5299,11 @@
       <c r="J133">
         <v>7138.02</v>
       </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" s="2">
@@ -4671,6 +5336,11 @@
       <c r="J134">
         <v>5633.3</v>
       </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" s="2">
@@ -4703,6 +5373,11 @@
       <c r="J135">
         <v>7259.139999999999</v>
       </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="136">
       <c r="A136" s="2">
@@ -4735,6 +5410,11 @@
       <c r="J136">
         <v>1171.94</v>
       </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" s="2">
@@ -4767,6 +5447,11 @@
       <c r="J137">
         <v>4145.77</v>
       </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="138">
       <c r="A138" s="2">
@@ -4799,6 +5484,11 @@
       <c r="J138">
         <v>330</v>
       </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="139">
       <c r="A139" s="2">
@@ -4831,6 +5521,11 @@
       <c r="J139">
         <v>16224.99</v>
       </c>
+      <c r="K139" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="140">
       <c r="A140" s="2">
@@ -4863,6 +5558,11 @@
       <c r="J140">
         <v>8510.4</v>
       </c>
+      <c r="K140" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="141">
       <c r="A141" s="2">
@@ -4895,6 +5595,11 @@
       <c r="J141">
         <v>4537.06</v>
       </c>
+      <c r="K141" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="142">
       <c r="A142" s="2">
@@ -4927,6 +5632,11 @@
       <c r="J142">
         <v>7292.469999999999</v>
       </c>
+      <c r="K142" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" s="2">
@@ -4959,6 +5669,11 @@
       <c r="J143">
         <v>3917.7</v>
       </c>
+      <c r="K143" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" s="2">
@@ -4991,6 +5706,11 @@
       <c r="J144">
         <v>3583.28</v>
       </c>
+      <c r="K144" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="145">
       <c r="A145" s="2">
@@ -5023,6 +5743,11 @@
       <c r="J145">
         <v>7065</v>
       </c>
+      <c r="K145" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="146">
       <c r="A146" s="2">
@@ -5055,6 +5780,11 @@
       <c r="J146">
         <v>4762.57</v>
       </c>
+      <c r="K146" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="147">
       <c r="A147" s="2">
@@ -5087,6 +5817,11 @@
       <c r="J147">
         <v>10314.26</v>
       </c>
+      <c r="K147" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="148">
       <c r="A148" s="2">
@@ -5119,6 +5854,11 @@
       <c r="J148">
         <v>6749.26</v>
       </c>
+      <c r="K148" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="149">
       <c r="A149" s="2">
@@ -5151,6 +5891,11 @@
       <c r="J149">
         <v>6208.429999999999</v>
       </c>
+      <c r="K149" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="150">
       <c r="A150" s="2">
@@ -5183,6 +5928,11 @@
       <c r="J150">
         <v>4396.77</v>
       </c>
+      <c r="K150" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="151">
       <c r="A151" s="2">
@@ -5215,6 +5965,11 @@
       <c r="J151">
         <v>1740</v>
       </c>
+      <c r="K151" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="152">
       <c r="A152" s="2">
@@ -5247,6 +6002,11 @@
       <c r="J152">
         <v>5319.01</v>
       </c>
+      <c r="K152" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="153">
       <c r="A153" s="2">
@@ -5279,6 +6039,11 @@
       <c r="J153">
         <v>3640.02</v>
       </c>
+      <c r="K153" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" s="2">
@@ -5311,6 +6076,11 @@
       <c r="J154">
         <v>4410.93</v>
       </c>
+      <c r="K154" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="155">
       <c r="A155" s="2">
@@ -5343,6 +6113,11 @@
       <c r="J155">
         <v>1532</v>
       </c>
+      <c r="K155" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" s="2">
@@ -5375,6 +6150,11 @@
       <c r="J156">
         <v>1928.9</v>
       </c>
+      <c r="K156" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" s="2">
@@ -5407,6 +6187,11 @@
       <c r="J157">
         <v>4239.66</v>
       </c>
+      <c r="K157" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="158">
       <c r="A158" s="2">
@@ -5439,6 +6224,11 @@
       <c r="J158">
         <v>6480.17</v>
       </c>
+      <c r="K158" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" s="2">
@@ -5471,6 +6261,11 @@
       <c r="J159">
         <v>7939.92</v>
       </c>
+      <c r="K159" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="160">
       <c r="A160" s="2">
@@ -5503,6 +6298,11 @@
       <c r="J160">
         <v>5186.42</v>
       </c>
+      <c r="K160" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="161">
       <c r="A161" s="2">
@@ -5535,6 +6335,11 @@
       <c r="J161">
         <v>9130</v>
       </c>
+      <c r="K161" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="162">
       <c r="A162" s="2">
@@ -5567,6 +6372,11 @@
       <c r="J162">
         <v>21903.61</v>
       </c>
+      <c r="K162" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="163">
       <c r="A163" s="2">
@@ -5599,6 +6409,11 @@
       <c r="J163">
         <v>7840</v>
       </c>
+      <c r="K163" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="164">
       <c r="A164" s="2">
@@ -5631,6 +6446,11 @@
       <c r="J164">
         <v>33407</v>
       </c>
+      <c r="K164" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" s="2">
@@ -5663,6 +6483,11 @@
       <c r="J165">
         <v>19998.91</v>
       </c>
+      <c r="K165" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="166">
       <c r="A166" s="2">
@@ -5695,6 +6520,11 @@
       <c r="J166">
         <v>9689.01</v>
       </c>
+      <c r="K166" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" s="2">
@@ -5727,6 +6557,11 @@
       <c r="J167">
         <v>980</v>
       </c>
+      <c r="K167" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="168">
       <c r="A168" s="2">
@@ -5759,6 +6594,11 @@
       <c r="J168">
         <v>6984</v>
       </c>
+      <c r="K168" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="169">
       <c r="A169" s="2">
@@ -5791,6 +6631,11 @@
       <c r="J169">
         <v>7220.74</v>
       </c>
+      <c r="K169" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="170">
       <c r="A170" s="2">
@@ -5823,6 +6668,11 @@
       <c r="J170">
         <v>4303.860000000001</v>
       </c>
+      <c r="K170" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="171">
       <c r="A171" s="2">
@@ -5855,6 +6705,11 @@
       <c r="J171">
         <v>20454.8</v>
       </c>
+      <c r="K171" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" s="2">
@@ -5887,6 +6742,11 @@
       <c r="J172">
         <v>1219.25</v>
       </c>
+      <c r="K172" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="173">
       <c r="A173" s="2">
@@ -5919,6 +6779,11 @@
       <c r="J173">
         <v>6775.33</v>
       </c>
+      <c r="K173" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="174">
       <c r="A174" s="2">
@@ -5951,6 +6816,11 @@
       <c r="J174">
         <v>3171.8</v>
       </c>
+      <c r="K174" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="175">
       <c r="A175" s="2">
@@ -5983,6 +6853,11 @@
       <c r="J175">
         <v>7123.8</v>
       </c>
+      <c r="K175" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="176">
       <c r="A176" s="2">
@@ -6015,6 +6890,11 @@
       <c r="J176">
         <v>15739.95</v>
       </c>
+      <c r="K176" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="177">
       <c r="A177" s="2">
@@ -6047,6 +6927,11 @@
       <c r="J177">
         <v>13645.31</v>
       </c>
+      <c r="K177" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="178">
       <c r="A178" s="2">
@@ -6079,6 +6964,11 @@
       <c r="J178">
         <v>8082.54</v>
       </c>
+      <c r="K178" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="179">
       <c r="A179" s="2">
@@ -6111,6 +7001,11 @@
       <c r="J179">
         <v>7800.96</v>
       </c>
+      <c r="K179" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" s="2">
@@ -6143,6 +7038,11 @@
       <c r="J180">
         <v>3603.7</v>
       </c>
+      <c r="K180" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" s="2">
@@ -6175,6 +7075,11 @@
       <c r="J181">
         <v>7657.139999999999</v>
       </c>
+      <c r="K181" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="182">
       <c r="A182" s="2">
@@ -6207,6 +7112,11 @@
       <c r="J182">
         <v>1793.7</v>
       </c>
+      <c r="K182" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" s="2">
@@ -6239,6 +7149,11 @@
       <c r="J183">
         <v>10601</v>
       </c>
+      <c r="K183" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" s="2">
@@ -6271,6 +7186,11 @@
       <c r="J184">
         <v>4914.780000000001</v>
       </c>
+      <c r="K184" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" s="2">
@@ -6303,6 +7223,11 @@
       <c r="J185">
         <v>11859.36</v>
       </c>
+      <c r="K185" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" s="2">
@@ -6335,6 +7260,11 @@
       <c r="J186">
         <v>66928.98</v>
       </c>
+      <c r="K186" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="187">
       <c r="A187" s="2">
@@ -6367,6 +7297,11 @@
       <c r="J187">
         <v>23987.97</v>
       </c>
+      <c r="K187" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="188">
       <c r="A188" s="2">
@@ -6399,6 +7334,11 @@
       <c r="J188">
         <v>17980.41</v>
       </c>
+      <c r="K188" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="189">
       <c r="A189" s="2">
@@ -6431,6 +7371,11 @@
       <c r="J189">
         <v>7639.94</v>
       </c>
+      <c r="K189" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="190">
       <c r="A190" s="2">
@@ -6463,6 +7408,11 @@
       <c r="J190">
         <v>12857.8</v>
       </c>
+      <c r="K190" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" s="2">
@@ -6495,6 +7445,11 @@
       <c r="J191">
         <v>3459.32</v>
       </c>
+      <c r="K191" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="192">
       <c r="A192" s="2">
@@ -6527,6 +7482,11 @@
       <c r="J192">
         <v>6605.4</v>
       </c>
+      <c r="K192" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="193">
       <c r="A193" s="2">
@@ -6559,6 +7519,11 @@
       <c r="J193">
         <v>150</v>
       </c>
+      <c r="K193" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="194">
       <c r="A194" s="2">
@@ -6591,6 +7556,11 @@
       <c r="J194">
         <v>2650</v>
       </c>
+      <c r="K194" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="195">
       <c r="A195" s="2">
@@ -6623,6 +7593,11 @@
       <c r="J195">
         <v>43090</v>
       </c>
+      <c r="K195" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="196">
       <c r="A196" s="2">
@@ -6655,6 +7630,11 @@
       <c r="J196">
         <v>87492.00999999999</v>
       </c>
+      <c r="K196" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" s="2">
@@ -6687,6 +7667,11 @@
       <c r="J197">
         <v>33369.62</v>
       </c>
+      <c r="K197" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" s="2">
@@ -6719,6 +7704,11 @@
       <c r="J198">
         <v>169995.24</v>
       </c>
+      <c r="K198" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="199">
       <c r="A199" s="2">
@@ -6751,6 +7741,11 @@
       <c r="J199">
         <v>11610.32</v>
       </c>
+      <c r="K199" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="200">
       <c r="A200" s="2">
@@ -6783,6 +7778,11 @@
       <c r="J200">
         <v>10465</v>
       </c>
+      <c r="K200" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="201">
       <c r="A201" s="2">
@@ -6815,6 +7815,11 @@
       <c r="J201">
         <v>9910</v>
       </c>
+      <c r="K201" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" s="2">
@@ -6847,6 +7852,11 @@
       <c r="J202">
         <v>5130</v>
       </c>
+      <c r="K202" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="203">
       <c r="A203" s="2">
@@ -6879,6 +7889,11 @@
       <c r="J203">
         <v>46909</v>
       </c>
+      <c r="K203" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="204">
       <c r="A204" s="2">
@@ -6911,6 +7926,11 @@
       <c r="J204">
         <v>200</v>
       </c>
+      <c r="K204" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="205">
       <c r="A205" s="2">
@@ -6943,6 +7963,11 @@
       <c r="J205">
         <v>3550</v>
       </c>
+      <c r="K205" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" s="2">
@@ -6975,6 +8000,11 @@
       <c r="J206">
         <v>16470</v>
       </c>
+      <c r="K206" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" s="2">
@@ -7007,6 +8037,11 @@
       <c r="J207">
         <v>6102.639999999999</v>
       </c>
+      <c r="K207" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" s="2">
@@ -7039,6 +8074,11 @@
       <c r="J208">
         <v>8390</v>
       </c>
+      <c r="K208" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="209">
       <c r="A209" s="2">
@@ -7071,6 +8111,11 @@
       <c r="J209">
         <v>6350</v>
       </c>
+      <c r="K209" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="210">
       <c r="A210" s="2">
@@ -7103,6 +8148,11 @@
       <c r="J210">
         <v>17127.39</v>
       </c>
+      <c r="K210" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="211">
       <c r="A211" s="2">
@@ -7135,6 +8185,11 @@
       <c r="J211">
         <v>11390.54</v>
       </c>
+      <c r="K211" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" s="2">
@@ -7167,6 +8222,11 @@
       <c r="J212">
         <v>31544</v>
       </c>
+      <c r="K212" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
     </row>
     <row r="213">
       <c r="A213" s="2">
@@ -7198,6 +8258,11 @@
       </c>
       <c r="J213">
         <v>25430.06</v>
+      </c>
+      <c r="K213" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
       </c>
     </row>
   </sheetData>
@@ -7488,13 +8553,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B8509D1-FBF4-48B2-8D56-A81F96B0B7AD}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DE0A735-DDD3-4FA2-95D0-EDA20D64E2DF}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{023920E8-8D64-4400-953E-41F7A0EAFA0A}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2E63297-C91A-4D8A-AF12-43ADBD594193}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74A5234D-6B67-435E-BB17-599926F5CC47}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD1CE6CF-6181-4B49-9E65-DD5FFE0E55C2}"/>
 </file>
</xml_diff>

<commit_message>
Scripts de pricing semanal 2015-2024 y pricing semanal histórico.
</commit_message>
<xml_diff>
--- a/Datos limpios/Pricing diario/2025/Cebada.xlsx
+++ b/Datos limpios/Pricing diario/2025/Cebada.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K213"/>
+  <dimension ref="A1:K219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8265,14 +8265,236 @@
         </is>
       </c>
     </row>
+    <row r="214">
+      <c r="A214" s="2">
+        <v>45950</v>
+      </c>
+      <c r="B214">
+        <v>25070</v>
+      </c>
+      <c r="C214">
+        <v>40</v>
+      </c>
+      <c r="D214">
+        <v>0</v>
+      </c>
+      <c r="E214">
+        <v>25110</v>
+      </c>
+      <c r="F214">
+        <v>4340</v>
+      </c>
+      <c r="G214">
+        <v>0</v>
+      </c>
+      <c r="H214">
+        <v>0</v>
+      </c>
+      <c r="I214">
+        <v>4340</v>
+      </c>
+      <c r="J214">
+        <v>29450</v>
+      </c>
+      <c r="K214" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="2">
+        <v>45951</v>
+      </c>
+      <c r="B215">
+        <v>32288.12</v>
+      </c>
+      <c r="C215">
+        <v>0</v>
+      </c>
+      <c r="D215">
+        <v>400</v>
+      </c>
+      <c r="E215">
+        <v>31888.12</v>
+      </c>
+      <c r="F215">
+        <v>500</v>
+      </c>
+      <c r="G215">
+        <v>0</v>
+      </c>
+      <c r="H215">
+        <v>0</v>
+      </c>
+      <c r="I215">
+        <v>500</v>
+      </c>
+      <c r="J215">
+        <v>32388.12</v>
+      </c>
+      <c r="K215" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="2">
+        <v>45952</v>
+      </c>
+      <c r="B216">
+        <v>23990.26</v>
+      </c>
+      <c r="C216">
+        <v>4240</v>
+      </c>
+      <c r="D216">
+        <v>0</v>
+      </c>
+      <c r="E216">
+        <v>28230.26</v>
+      </c>
+      <c r="F216">
+        <v>1500</v>
+      </c>
+      <c r="G216">
+        <v>0</v>
+      </c>
+      <c r="H216">
+        <v>0</v>
+      </c>
+      <c r="I216">
+        <v>1500</v>
+      </c>
+      <c r="J216">
+        <v>29730.26</v>
+      </c>
+      <c r="K216" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="2">
+        <v>45953</v>
+      </c>
+      <c r="B217">
+        <v>10986</v>
+      </c>
+      <c r="C217">
+        <v>500</v>
+      </c>
+      <c r="D217">
+        <v>0</v>
+      </c>
+      <c r="E217">
+        <v>11486</v>
+      </c>
+      <c r="F217">
+        <v>30</v>
+      </c>
+      <c r="G217">
+        <v>0</v>
+      </c>
+      <c r="H217">
+        <v>0</v>
+      </c>
+      <c r="I217">
+        <v>30</v>
+      </c>
+      <c r="J217">
+        <v>11516</v>
+      </c>
+      <c r="K217" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="2">
+        <v>45954</v>
+      </c>
+      <c r="B218">
+        <v>14826.67</v>
+      </c>
+      <c r="C218">
+        <v>710</v>
+      </c>
+      <c r="D218">
+        <v>0</v>
+      </c>
+      <c r="E218">
+        <v>15536.67</v>
+      </c>
+      <c r="F218">
+        <v>51.18000000000001</v>
+      </c>
+      <c r="G218">
+        <v>0</v>
+      </c>
+      <c r="H218">
+        <v>0</v>
+      </c>
+      <c r="I218">
+        <v>51.18000000000001</v>
+      </c>
+      <c r="J218">
+        <v>15587.85</v>
+      </c>
+      <c r="K218" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="2">
+        <v>45957</v>
+      </c>
+      <c r="B219">
+        <v>450</v>
+      </c>
+      <c r="C219">
+        <v>0</v>
+      </c>
+      <c r="D219">
+        <v>0</v>
+      </c>
+      <c r="E219">
+        <v>450</v>
+      </c>
+      <c r="F219">
+        <v>7500</v>
+      </c>
+      <c r="G219">
+        <v>0</v>
+      </c>
+      <c r="H219">
+        <v>0</v>
+      </c>
+      <c r="I219">
+        <v>7500</v>
+      </c>
+      <c r="J219">
+        <v>7950</v>
+      </c>
+      <c r="K219" t="inlineStr">
+        <is>
+          <t>CEBADA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D6CA5EAACE9DA04D9E421A617A76D009" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="bac5de4a034fee97af64ba5a2822cd53">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="77131357-5c03-45fa-a80b-b9111bb46cb1" xmlns:ns3="d3f11db4-a96c-41b4-b8ec-902c72f52048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="027d3429df443898fbbc0b888682b5bf" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100D6CA5EAACE9DA04D9E421A617A76D009" ma:contentTypeVersion="19" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="854b0670eee28d8fa271d4f22cb9c97d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="77131357-5c03-45fa-a80b-b9111bb46cb1" xmlns:ns3="d3f11db4-a96c-41b4-b8ec-902c72f52048" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b486ba09ce8a2fb19cc660d7edf32df4" ns2:_="" ns3:_="">
     <xsd:import namespace="77131357-5c03-45fa-a80b-b9111bb46cb1"/>
     <xsd:import namespace="d3f11db4-a96c-41b4-b8ec-902c72f52048"/>
     <xsd:element name="properties">
@@ -8553,13 +8775,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3DE0A735-DDD3-4FA2-95D0-EDA20D64E2DF}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75BCCBBD-C199-48BF-B4C3-DEF88CEA1AF0}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A2E63297-C91A-4D8A-AF12-43ADBD594193}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D610BE4-1CCB-4D61-BE40-34DFEA472844}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD1CE6CF-6181-4B49-9E65-DD5FFE0E55C2}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{625EC8D6-C9D5-4C65-A18C-5509193A5453}"/>
 </file>
</xml_diff>